<commit_message>
новый файл:    .gitignore 	изменено:      Dockerfile 	изменено:      README.md 	новый файл:    data/.env.template 	изменено:      data/actual_table.xlsx 	изменено:      data/log.log 	изменено:      data/req_archive.xlsx 	изменено:      requirements.txt
</commit_message>
<xml_diff>
--- a/data/actual_table.xlsx
+++ b/data/actual_table.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="62">
   <si>
     <t>Номер</t>
   </si>
@@ -92,10 +92,74 @@
     <t>Информация о закрытии</t>
   </si>
   <si>
-    <t>REQ0683527</t>
-  </si>
-  <si>
-    <t>SUTSPROD-9619515</t>
+    <t>REQ0717399</t>
+  </si>
+  <si>
+    <t>Тетерев
+pax d270
++78345340618
+адрес-гагарина 36
+Нужна замена сим-карты у нее билайн</t>
+  </si>
+  <si>
+    <t>on_hold</t>
+  </si>
+  <si>
+    <t>2024-10-27 15:25:32</t>
+  </si>
+  <si>
+    <t>2024-10-30 08:43:15</t>
+  </si>
+  <si>
+    <t>431350, Респ Мордовия, г Ковылкино, ул Гагарина, д 36</t>
+  </si>
+  <si>
+    <t>Холопов Александр Сергеевич</t>
+  </si>
+  <si>
+    <t>REQ0715319</t>
+  </si>
+  <si>
+    <t>Заявка на демонтаж</t>
+  </si>
+  <si>
+    <t>2024-10-25 16:43:18</t>
+  </si>
+  <si>
+    <t>2024-10-26 16:43:13</t>
+  </si>
+  <si>
+    <t>набрать с понедельника</t>
+  </si>
+  <si>
+    <t>г Саранск, ул Пролетарская, д 130А</t>
+  </si>
+  <si>
+    <t>430001, Респ Мордовия, г Саранск, ул Пролетарская, д 130А</t>
+  </si>
+  <si>
+    <t>REQ0714742</t>
+  </si>
+  <si>
+    <t>Заявка на установку терминала</t>
+  </si>
+  <si>
+    <t>2024-10-25 15:15:16</t>
+  </si>
+  <si>
+    <t>2024-10-26 15:15:11</t>
+  </si>
+  <si>
+    <t>позвонить 30.10 до обеда. (терминал готов)</t>
+  </si>
+  <si>
+    <t>430034, Респ Мордовия, г Саранск, Лямбирское шоссе, д 12</t>
+  </si>
+  <si>
+    <t>REQ0714563</t>
+  </si>
+  <si>
+    <t>SUTSPROD-9689074</t>
   </si>
   <si>
     <t>expertise</t>
@@ -104,189 +168,61 @@
     <t>in_progress</t>
   </si>
   <si>
-    <t>2024-10-15 14:05:39</t>
-  </si>
-  <si>
-    <t>2024-10-22 14:05:37</t>
-  </si>
-  <si>
-    <t>W0216842</t>
-  </si>
-  <si>
-    <t>Номер заявки Мультикарты: SUTSPROD-9619515
+    <t>2024-10-25 14:51:05</t>
+  </si>
+  <si>
+    <t>2024-11-01 14:51:02</t>
+  </si>
+  <si>
+    <t>00018537558</t>
+  </si>
+  <si>
+    <t>00011211594</t>
+  </si>
+  <si>
+    <t>W0132418</t>
+  </si>
+  <si>
+    <t>Номер заявки Мультикарты: SUTSPROD-9689074
 Принадлежность оборудования по заявке: Информация остутствует
 Серийный номер демонтируемого ТО: Информация остутствует
 Серийный номер демонтируемого PIN: Информация остутствует
-Производитель устанавливаемого ТО: pax
+Производитель устанавливаемого ТО: aisino
 Модель устанавливаемого ТО: Информация остутствует
-Тип устанавливаемого ТО: portable_pos
+Тип устанавливаемого ТО: stat_pos
 Дата и время согласованного доступа: Информация остутствует
 Тип заявки: expertise
-Категория обслуживания: premium_kto_1
+Категория обслуживания: standart_kto_1
 Город склада: Саранск
 Адрес установки терминала: Информация остутствует
 Заказчик: Информация остутствует
-Оборудование POS: 2331822914
-Оборудование Pin Pad: Информация остутствует
+Оборудование POS: 00018537558
+Оборудование Pin Pad: 00011211594
 Доп. информация: 0
 ID СБП: Информация остутствует
 ИНН ТСП: Информация остутствует
 Комментарий к результату выезда: Информация остутствует</t>
   </si>
   <si>
-    <t>Савин Даниил Андреевич</t>
+    <t>Бикмурзин Айнур Ренатович</t>
   </si>
   <si>
     <t>Щеглов Виктор Александрович</t>
   </si>
   <si>
-    <t>REQ0683441</t>
-  </si>
-  <si>
-    <t>SUTSPROD-9619391</t>
-  </si>
-  <si>
-    <t>2024-10-15 13:51:46</t>
-  </si>
-  <si>
-    <t>2024-10-22 13:51:44</t>
-  </si>
-  <si>
-    <t>W0174163</t>
-  </si>
-  <si>
-    <t>Номер заявки Мультикарты: SUTSPROD-9619391
-Принадлежность оборудования по заявке: Информация остутствует
-Серийный номер демонтируемого ТО: Информация остутствует
-Серийный номер демонтируемого PIN: Информация остутствует
-Производитель устанавливаемого ТО: pax
-Модель устанавливаемого ТО: Информация остутствует
-Тип устанавливаемого ТО: portable_pos
-Дата и время согласованного доступа: Информация остутствует
-Тип заявки: expertise
-Категория обслуживания: premium_kto_1
-Город склада: Саранск
-Адрес установки терминала: Информация остутствует
-Заказчик: Информация остутствует
-Оборудование POS: 2331428123
-Оборудование Pin Pad: Информация остутствует
-Доп. информация: 0
-ID СБП: Информация остутствует
-ИНН ТСП: Информация остутствует
-Комментарий к результату выезда: Информация остутствует</t>
-  </si>
-  <si>
-    <t>REQ0683303</t>
-  </si>
-  <si>
-    <t>SUTSPROD-9619138</t>
-  </si>
-  <si>
-    <t>replacement</t>
-  </si>
-  <si>
-    <t>2024-10-15 13:22:39</t>
-  </si>
-  <si>
-    <t>2024-10-17 13:22:37</t>
-  </si>
-  <si>
-    <t>Поселок Кадошкино, ул. Заводская, 12А</t>
-  </si>
-  <si>
-    <t>W0118530</t>
-  </si>
-  <si>
-    <t>aisino</t>
-  </si>
-  <si>
-    <t>IP Plaksina A.V.</t>
-  </si>
-  <si>
-    <t>Номер заявки Мультикарты: SUTSPROD-9619138
-Принадлежность оборудования по заявке: SMB
-Серийный номер демонтируемого ТО: 00018537347
-Серийный номер демонтируемого PIN: Информация остутствует
-Производитель устанавливаемого ТО: pax
-Модель устанавливаемого ТО: D230 4G BT WIFI ETH CTLS Camera+NFC TAG
-Тип устанавливаемого ТО: stat_pos
-Дата и время согласованного доступа: Информация остутствует
-Тип заявки: replacement
-Категория обслуживания: standart_kto_1
-Город склада: Саранск
-Адрес установки терминала: Поселок Кадошкино, ул. Заводская, 12А
-Заказчик: Информация остутствует
-Оборудование POS: 2331807086
-Оборудование Pin Pad: Информация остутствует
-Доп. информация: null Выключается терминал; СМЕНА КЛЮЧЕЙ ПО ЗВОНКУ, Ближайшая дата обеспечения доступа: уточнить самостоятельно звонком. Режим обслуживания: 7*12. ; Терминал работает! Прошу сохранить работоспособность.; ;  (10.15  12:40:49 Направлена через СУТС) All Клиент просит заменить
-ID СБП: Информация остутствует
-ИНН ТСП: 131100189586</t>
-  </si>
-  <si>
-    <t>null Выключается терминал; СМЕНА КЛЮЧЕЙ ПО ЗВОНКУ, Ближайшая дата обеспечения доступа: уточнить самостоятельно звонком. Режим обслуживания: 7*12. ; Терминал работает! Прошу сохранить работоспособность.; ;  (10.15  12:40:49 Направлена через СУТС) All Клиент просит заменить</t>
-  </si>
-  <si>
-    <t>Астафьев Вячеслав Васильевич</t>
-  </si>
-  <si>
-    <t>REQ0683077</t>
-  </si>
-  <si>
-    <t>Заявка на установку терминала</t>
-  </si>
-  <si>
-    <t>on_hold</t>
-  </si>
-  <si>
-    <t>2024-10-15 12:41:55</t>
-  </si>
-  <si>
-    <t>2024-10-16 12:41:52</t>
-  </si>
-  <si>
-    <t>поставить до 18.10 терминал готов</t>
-  </si>
-  <si>
-    <t>Калдоркин</t>
-  </si>
-  <si>
-    <t>431890, Респ Мордовия, Ардатовский р-н, рп Тургенево, ул Воробьевка, д 19</t>
-  </si>
-  <si>
-    <t>REQ0679856</t>
-  </si>
-  <si>
-    <t>2024-10-14 13:15:34</t>
-  </si>
-  <si>
-    <t>2024-11-01 09:44:42</t>
-  </si>
-  <si>
-    <t>не абонент, но завтра сделаем!</t>
-  </si>
-  <si>
-    <t>430014, Респ Мордовия, г Саранск, ул Волгоградская, д 71</t>
-  </si>
-  <si>
-    <t>REQ0561303</t>
-  </si>
-  <si>
-    <t>Заявка на демонтаж</t>
-  </si>
-  <si>
-    <t>2024-09-02 14:55:32</t>
-  </si>
-  <si>
-    <t>2024-11-01 00:20:44</t>
-  </si>
-  <si>
-    <t>Клиент в больнице. Перезвонит по возможности вернуть ТО. (ожидаем звонка)</t>
-  </si>
-  <si>
-    <t>Респ Мордовия, Чамзинский р-н, рп Комсомольский, ул Республиканская, д 47</t>
-  </si>
-  <si>
-    <t>431720, Республика Мордовия, Чамзинский р-н, рп Комсомольский, ул Республиканская, д 47</t>
+    <t>REQ0714396</t>
+  </si>
+  <si>
+    <t>2024-10-25 14:15:24</t>
+  </si>
+  <si>
+    <t>2024-10-28 15:40:02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Выезд согласован на понедельник с 9 до 12. Терминал готов. </t>
+  </si>
+  <si>
+    <t>430005, Респ Мордовия, г Саранск, ул Коммунистическая, д 25</t>
   </si>
 </sst>
 </file>
@@ -625,7 +561,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:Y7"/>
+  <dimension ref="A1:Y6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -717,179 +653,171 @@
       <c r="B2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2"/>
+      <c r="D2" t="s">
         <v>27</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>28</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>29</v>
-      </c>
-      <c r="F2" t="s">
-        <v>30</v>
       </c>
       <c r="G2"/>
       <c r="H2"/>
       <c r="I2"/>
-      <c r="J2">
-        <v>2331822914</v>
-      </c>
+      <c r="J2"/>
       <c r="K2"/>
-      <c r="L2" t="s">
-        <v>31</v>
-      </c>
+      <c r="L2"/>
       <c r="M2"/>
       <c r="N2"/>
       <c r="O2"/>
       <c r="P2"/>
       <c r="Q2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="R2"/>
-      <c r="S2" t="s">
-        <v>33</v>
-      </c>
+      <c r="S2"/>
       <c r="T2"/>
-      <c r="U2"/>
+      <c r="U2" t="s">
+        <v>30</v>
+      </c>
       <c r="V2"/>
       <c r="W2" t="s">
-        <v>34</v>
-      </c>
-      <c r="X2"/>
+        <v>31</v>
+      </c>
+      <c r="X2">
+        <v>92260524</v>
+      </c>
       <c r="Y2"/>
     </row>
     <row r="3" spans="1:25">
       <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3"/>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" t="s">
         <v>35</v>
-      </c>
-      <c r="B3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" t="s">
-        <v>38</v>
       </c>
       <c r="G3"/>
       <c r="H3"/>
-      <c r="I3"/>
-      <c r="J3">
-        <v>2331428123</v>
-      </c>
+      <c r="I3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3"/>
       <c r="K3"/>
-      <c r="L3" t="s">
-        <v>39</v>
-      </c>
+      <c r="L3"/>
       <c r="M3"/>
       <c r="N3"/>
       <c r="O3"/>
       <c r="P3"/>
       <c r="Q3" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="R3"/>
-      <c r="S3" t="s">
-        <v>33</v>
-      </c>
-      <c r="T3"/>
-      <c r="U3"/>
+      <c r="S3"/>
+      <c r="T3" t="s">
+        <v>37</v>
+      </c>
+      <c r="U3" t="s">
+        <v>38</v>
+      </c>
       <c r="V3"/>
       <c r="W3" t="s">
-        <v>34</v>
-      </c>
-      <c r="X3"/>
+        <v>31</v>
+      </c>
+      <c r="X3">
+        <v>92638972</v>
+      </c>
       <c r="Y3"/>
     </row>
     <row r="4" spans="1:25">
       <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4"/>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
         <v>41</v>
       </c>
-      <c r="B4" t="s">
+      <c r="F4" t="s">
         <v>42</v>
       </c>
-      <c r="C4" t="s">
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4" t="s">
         <v>43</v>
       </c>
-      <c r="D4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G4"/>
-      <c r="H4" t="s">
-        <v>46</v>
-      </c>
-      <c r="I4"/>
-      <c r="J4">
-        <v>2331807086</v>
-      </c>
+      <c r="J4"/>
       <c r="K4"/>
-      <c r="L4" t="s">
-        <v>47</v>
-      </c>
+      <c r="L4"/>
       <c r="M4"/>
       <c r="N4"/>
-      <c r="O4" t="s">
-        <v>48</v>
-      </c>
-      <c r="P4" t="s">
-        <v>49</v>
-      </c>
+      <c r="O4"/>
+      <c r="P4"/>
       <c r="Q4" t="s">
-        <v>50</v>
-      </c>
-      <c r="R4" t="s">
-        <v>51</v>
-      </c>
-      <c r="S4" t="s">
-        <v>52</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="R4"/>
+      <c r="S4"/>
       <c r="T4"/>
-      <c r="U4"/>
+      <c r="U4" t="s">
+        <v>44</v>
+      </c>
       <c r="V4"/>
       <c r="W4" t="s">
-        <v>34</v>
-      </c>
-      <c r="X4"/>
+        <v>31</v>
+      </c>
+      <c r="X4">
+        <v>93424991</v>
+      </c>
       <c r="Y4"/>
     </row>
     <row r="5" spans="1:25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5"/>
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="G5"/>
       <c r="H5"/>
-      <c r="I5" t="s">
-        <v>58</v>
-      </c>
-      <c r="J5"/>
-      <c r="K5"/>
-      <c r="L5"/>
+      <c r="I5"/>
+      <c r="J5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L5" t="s">
+        <v>53</v>
+      </c>
       <c r="M5"/>
       <c r="N5"/>
       <c r="O5"/>
@@ -897,44 +825,40 @@
       <c r="Q5" t="s">
         <v>54</v>
       </c>
-      <c r="R5" t="s">
-        <v>59</v>
-      </c>
-      <c r="S5"/>
+      <c r="R5"/>
+      <c r="S5" t="s">
+        <v>55</v>
+      </c>
       <c r="T5"/>
-      <c r="U5" t="s">
-        <v>60</v>
-      </c>
+      <c r="U5"/>
       <c r="V5"/>
       <c r="W5" t="s">
-        <v>52</v>
-      </c>
-      <c r="X5">
-        <v>93399054</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="X5"/>
       <c r="Y5"/>
     </row>
     <row r="6" spans="1:25">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C6"/>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G6"/>
       <c r="H6"/>
       <c r="I6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="J6"/>
       <c r="K6"/>
@@ -944,73 +868,22 @@
       <c r="O6"/>
       <c r="P6"/>
       <c r="Q6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="R6"/>
       <c r="S6"/>
       <c r="T6"/>
       <c r="U6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="V6"/>
       <c r="W6" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="X6">
-        <v>93397591</v>
+        <v>93424698</v>
       </c>
       <c r="Y6"/>
-    </row>
-    <row r="7" spans="1:25">
-      <c r="A7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C7"/>
-      <c r="D7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F7" t="s">
-        <v>69</v>
-      </c>
-      <c r="G7"/>
-      <c r="H7"/>
-      <c r="I7" t="s">
-        <v>70</v>
-      </c>
-      <c r="J7"/>
-      <c r="K7"/>
-      <c r="L7"/>
-      <c r="M7"/>
-      <c r="N7"/>
-      <c r="O7"/>
-      <c r="P7"/>
-      <c r="Q7" t="s">
-        <v>67</v>
-      </c>
-      <c r="R7" t="s">
-        <v>59</v>
-      </c>
-      <c r="S7"/>
-      <c r="T7" t="s">
-        <v>71</v>
-      </c>
-      <c r="U7" t="s">
-        <v>72</v>
-      </c>
-      <c r="V7"/>
-      <c r="W7" t="s">
-        <v>52</v>
-      </c>
-      <c r="X7">
-        <v>92506313</v>
-      </c>
-      <c r="Y7"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>